<commit_message>
Minor history fetching and admin excel uploading bug fixing...
</commit_message>
<xml_diff>
--- a/admin/assets/station_sample.xlsx
+++ b/admin/assets/station_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arshil's workplace\Sem-6\project_e_ticket_management_system\admin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0389CEFC-F0AB-44FB-8EC9-B1BA8896070E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A39908D-6B2C-4ECA-935A-2A38A0A68311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{6D95A40A-27EC-4D1E-9A2B-0758742EF803}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Station ID</t>
   </si>
@@ -63,6 +63,54 @@
   </si>
   <si>
     <t>Kalakunj Society</t>
+  </si>
+  <si>
+    <t>Seven Star Residency</t>
+  </si>
+  <si>
+    <t>VNSGU</t>
+  </si>
+  <si>
+    <t>Sarthana Nature Park</t>
+  </si>
+  <si>
+    <t>Maharana Partap Garden</t>
+  </si>
+  <si>
+    <t>Adajan Patiya</t>
+  </si>
+  <si>
+    <t>Gujrat Gas Circle</t>
+  </si>
+  <si>
+    <t>Athva Gate</t>
+  </si>
+  <si>
+    <t>Majura Gate</t>
+  </si>
+  <si>
+    <t>Surat Railway Station</t>
+  </si>
+  <si>
+    <t>Gotalavadi</t>
+  </si>
+  <si>
+    <t>Kiran Hospital</t>
+  </si>
+  <si>
+    <t>Vallabhacharya RD</t>
+  </si>
+  <si>
+    <t>Hirabaug Circle</t>
+  </si>
+  <si>
+    <t>Kapodra Fire Station</t>
+  </si>
+  <si>
+    <t>Yogi Nagar Brts</t>
+  </si>
+  <si>
+    <t>Simada Canal Junc.</t>
   </si>
 </sst>
 </file>
@@ -423,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE2B7CE-B64C-4153-8220-B42784CAB2E8}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,6 +569,230 @@
         <v>72.875692000000001</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2000</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>21.245918</v>
+      </c>
+      <c r="D7">
+        <v>72.861221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7438</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>21.153851</v>
+      </c>
+      <c r="D8">
+        <v>72.779714999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>473</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>21.229827</v>
+      </c>
+      <c r="D9">
+        <v>72.899540999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8493</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>21.224121</v>
+      </c>
+      <c r="D10">
+        <v>72.884878</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9843</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>21.198701</v>
+      </c>
+      <c r="D11">
+        <v>72.807055000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>8372</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>21.193932</v>
+      </c>
+      <c r="D12">
+        <v>72.801903999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>6582</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>21.185621000000001</v>
+      </c>
+      <c r="D13">
+        <v>72.810660999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>7461</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>21.180719</v>
+      </c>
+      <c r="D14">
+        <v>72.818521000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>4781</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>21.204922</v>
+      </c>
+      <c r="D15">
+        <v>72.839980999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>3213</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>21.211634</v>
+      </c>
+      <c r="D16">
+        <v>72.830855999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>8664</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>21.219275</v>
+      </c>
+      <c r="D17">
+        <v>72.837095000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>9823</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>21.219588000000002</v>
+      </c>
+      <c r="D18">
+        <v>72.851616000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>9503</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>21.215689000000001</v>
+      </c>
+      <c r="D19">
+        <v>72.862960999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>8872</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>21.220329</v>
+      </c>
+      <c r="D20">
+        <v>72.874052000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2032</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>21.217689</v>
+      </c>
+      <c r="D21">
+        <v>72.895975000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>7463</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>21.210167999999999</v>
+      </c>
+      <c r="D22">
+        <v>72.896876000000006</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>